<commit_message>
ran odds, other fixes
</commit_message>
<xml_diff>
--- a/data/odds calc.xlsx
+++ b/data/odds calc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahedges\Documents\Personal\Sports &amp; Stats\Fantasy Football\2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\football\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{718E248E-02B1-4CB8-B879-D47315A638E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72D6846-B62C-42A9-9BD6-B7C7251516C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="18000" windowHeight="8988" xr2:uid="{C3C2C1FA-070B-4845-B992-F8F721B1F198}"/>
+    <workbookView xWindow="6120" yWindow="1913" windowWidth="19200" windowHeight="10214" xr2:uid="{C3C2C1FA-070B-4845-B992-F8F721B1F198}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 10" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <sheet name="Probablities" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -726,20 +725,20 @@
   <dimension ref="B1:W19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="6" max="9" width="9.28515625" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="3.28515625" customWidth="1"/>
-    <col min="17" max="17" width="2.28515625" customWidth="1"/>
-    <col min="21" max="22" width="2.5703125" customWidth="1"/>
+    <col min="6" max="9" width="9.29296875" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="12.29296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="9.1171875" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="3.29296875" customWidth="1"/>
+    <col min="17" max="17" width="2.29296875" customWidth="1"/>
+    <col min="21" max="22" width="2.5859375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:23" x14ac:dyDescent="0.5">
       <c r="D1" s="4" t="s">
         <v>0</v>
       </c>
@@ -762,7 +761,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -814,7 +813,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B3" s="3" t="s">
         <v>29</v>
       </c>
@@ -882,15 +881,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="3">
-        <v>-3</v>
+      <c r="D4">
+        <v>-2.5</v>
       </c>
       <c r="E4">
         <v>-2</v>
@@ -901,7 +900,7 @@
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="H4" t="b">
         <f>IF(D4&lt;0,IF(D4&lt;-7.5,B4,FALSE),IF(AND(D4&gt;3.5,D4&lt;7),B4,FALSE))</f>
@@ -921,11 +920,11 @@
       </c>
       <c r="L4" t="str" cm="1">
         <f t="array" ref="L4">_xlfn.IFS(E4=D4,"No MOV",E4&lt;=0,IF(E4&lt;D4,B4&amp;" "&amp;(D4-E4),C4&amp;" "&amp;(D4-E4)),E4&gt;0,IF(E4&lt;D4,B4&amp;" "&amp;(E4-D4),C4&amp;" "&amp;(E4-D4)))</f>
-        <v>Browns -1</v>
+        <v>Browns -0.5</v>
       </c>
       <c r="M4" cm="1">
         <f t="array" ref="M4">_xlfn.IFS(E4=D4,"No MOV",E4&lt;0,IF(E4&lt;D4,(D4-E4),(D4-E4)),E4&gt;0,IF(E4&lt;D4,(E4-D4),(E4-D4)))</f>
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="N4" t="str" cm="1">
         <f t="array" ref="N4">IF(J4&lt;&gt;K4,_xlfn.IFS(M4&gt;0,"MAYBE",M4&lt;0,"IGNORE"),"")</f>
@@ -939,14 +938,14 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5">
         <v>-1.5</v>
       </c>
       <c r="E5">
@@ -996,14 +995,14 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6">
         <v>10.5</v>
       </c>
       <c r="E6">
@@ -1050,15 +1049,15 @@
         <v>Steelers</v>
       </c>
     </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="3">
-        <v>-1.5</v>
+      <c r="D7">
+        <v>-1</v>
       </c>
       <c r="E7">
         <v>-3</v>
@@ -1069,7 +1068,7 @@
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="H7" t="b">
         <f>IF(D7&lt;0,IF(D7&lt;-7.5,C7,FALSE),IF(AND(D7&gt;3.5,D7&lt;7),C7,FALSE))</f>
@@ -1089,11 +1088,11 @@
       </c>
       <c r="L7" t="str" cm="1">
         <f t="array" ref="L7">_xlfn.IFS(E7=D7,"No MOV",E7&lt;=0,IF(E7&lt;D7,B7&amp;" "&amp;(D7-E7),C7&amp;" "&amp;(D7-E7)),E7&gt;0,IF(E7&lt;D7,B7&amp;" "&amp;(E7-D7),C7&amp;" "&amp;(E7-D7)))</f>
-        <v>Lions 1.5</v>
+        <v>Lions 2</v>
       </c>
       <c r="M7" cm="1">
         <f t="array" ref="M7">_xlfn.IFS(E7=D7,"No MOV",E7&lt;0,IF(E7&lt;D7,(D7-E7),(D7-E7)),E7&gt;0,IF(E7&lt;D7,(E7-D7),(E7-D7)))</f>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="N7" t="str" cm="1">
         <f t="array" ref="N7">IF(J7&lt;&gt;K7,_xlfn.IFS(M7&gt;0,"MAYBE",M7&lt;0,"IGNORE"),"")</f>
@@ -1104,15 +1103,15 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="3">
-        <v>-5</v>
+      <c r="D8">
+        <v>-6</v>
       </c>
       <c r="E8">
         <v>-6.5</v>
@@ -1123,7 +1122,7 @@
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H8" t="b">
         <f>IF(D8&lt;0,IF(D8&lt;-7.5,C8,FALSE),IF(AND(D8&gt;3.5,D8&lt;7),C8,FALSE))</f>
@@ -1143,11 +1142,11 @@
       </c>
       <c r="L8" t="str" cm="1">
         <f t="array" ref="L8">_xlfn.IFS(E8=D8,"No MOV",E8&lt;=0,IF(E8&lt;D8,B8&amp;" "&amp;(D8-E8),C8&amp;" "&amp;(D8-E8)),E8&gt;0,IF(E8&lt;D8,B8&amp;" "&amp;(E8-D8),C8&amp;" "&amp;(E8-D8)))</f>
-        <v>Titans 1.5</v>
+        <v>Titans 0.5</v>
       </c>
       <c r="M8" cm="1">
         <f t="array" ref="M8">_xlfn.IFS(E8=D8,"No MOV",E8&lt;0,IF(E8&lt;D8,(D8-E8),(D8-E8)),E8&gt;0,IF(E8&lt;D8,(E8-D8),(E8-D8)))</f>
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="N8" t="str" cm="1">
         <f t="array" ref="N8">IF(J8&lt;&gt;K8,_xlfn.IFS(M8&gt;0,"MAYBE",M8&lt;0,"IGNORE"),"")</f>
@@ -1158,15 +1157,15 @@
         <v>Titans</v>
       </c>
     </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B9" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="3">
-        <v>-4</v>
+      <c r="D9">
+        <v>-3.5</v>
       </c>
       <c r="E9">
         <v>-7</v>
@@ -1177,7 +1176,7 @@
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="H9" t="b">
         <f>IF(D9&lt;0,IF(D9&lt;-7.5,#REF!,FALSE),IF(AND(D9&gt;3.5,D9&lt;7),#REF!,FALSE))</f>
@@ -1197,11 +1196,11 @@
       </c>
       <c r="L9" t="str" cm="1">
         <f t="array" ref="L9">_xlfn.IFS(E9=D9,"No MOV",E9&lt;=0,IF(E9&lt;D9,B9&amp;" "&amp;(D9-E9),C9&amp;" "&amp;(D9-E9)),E9&gt;0,IF(E9&lt;D9,B9&amp;" "&amp;(E9-D9),C9&amp;" "&amp;(E9-D9)))</f>
-        <v>Falcons 3</v>
+        <v>Falcons 3.5</v>
       </c>
       <c r="M9" cm="1">
         <f t="array" ref="M9">_xlfn.IFS(E9=D9,"No MOV",E9&lt;0,IF(E9&lt;D9,(D9-E9),(D9-E9)),E9&gt;0,IF(E9&lt;D9,(E9-D9),(E9-D9)))</f>
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="N9" t="str" cm="1">
         <f t="array" ref="N9">IF(J9&lt;&gt;K9,_xlfn.IFS(M9&gt;0,"MAYBE",M9&lt;0,"IGNORE"),"")</f>
@@ -1212,14 +1211,14 @@
         <v>Falcons</v>
       </c>
     </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B10" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10">
         <v>2</v>
       </c>
       <c r="E10">
@@ -1266,15 +1265,15 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B11" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="3">
-        <v>3.5</v>
+      <c r="D11">
+        <v>4</v>
       </c>
       <c r="E11">
         <v>-1</v>
@@ -1285,11 +1284,11 @@
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
-        <v>-3.5</v>
-      </c>
-      <c r="H11" t="b">
+        <v>-4</v>
+      </c>
+      <c r="H11" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>Broncos</v>
       </c>
       <c r="I11" t="b">
         <f t="shared" si="5"/>
@@ -1305,11 +1304,11 @@
       </c>
       <c r="L11" t="str" cm="1">
         <f t="array" ref="L11">_xlfn.IFS(E11=D11,"No MOV",E11&lt;=0,IF(E11&lt;D11,B11&amp;" "&amp;(D11-E11),C11&amp;" "&amp;(D11-E11)),E11&gt;0,IF(E11&lt;D11,B11&amp;" "&amp;(E11-D11),C11&amp;" "&amp;(E11-D11)))</f>
-        <v>Dolphins 4.5</v>
+        <v>Dolphins 5</v>
       </c>
       <c r="M11" cm="1">
         <f t="array" ref="M11">_xlfn.IFS(E11=D11,"No MOV",E11&lt;0,IF(E11&lt;D11,(D11-E11),(D11-E11)),E11&gt;0,IF(E11&lt;D11,(E11-D11),(E11-D11)))</f>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="N11" t="str" cm="1">
         <f t="array" ref="N11">IF(J11&lt;&gt;K11,_xlfn.IFS(M11&gt;0,"MAYBE",M11&lt;0,"IGNORE"),"")</f>
@@ -1323,15 +1322,15 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B12" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="3">
-        <v>-9</v>
+      <c r="D12">
+        <v>-10</v>
       </c>
       <c r="E12">
         <v>-8.5</v>
@@ -1342,7 +1341,7 @@
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="4"/>
@@ -1362,11 +1361,11 @@
       </c>
       <c r="L12" t="str" cm="1">
         <f t="array" ref="L12">_xlfn.IFS(E12=D12,"No MOV",E12&lt;=0,IF(E12&lt;D12,B12&amp;" "&amp;(D12-E12),C12&amp;" "&amp;(D12-E12)),E12&gt;0,IF(E12&lt;D12,B12&amp;" "&amp;(E12-D12),C12&amp;" "&amp;(E12-D12)))</f>
-        <v>Chargers -0.5</v>
+        <v>Chargers -1.5</v>
       </c>
       <c r="M12" cm="1">
         <f t="array" ref="M12">_xlfn.IFS(E12=D12,"No MOV",E12&lt;0,IF(E12&lt;D12,(D12-E12),(D12-E12)),E12&gt;0,IF(E12&lt;D12,(E12-D12),(E12-D12)))</f>
-        <v>-0.5</v>
+        <v>-1.5</v>
       </c>
       <c r="N12" t="str" cm="1">
         <f t="array" ref="N12">IF(J12&lt;&gt;K12,_xlfn.IFS(M12&gt;0,"MAYBE",M12&lt;0,"IGNORE"),"")</f>
@@ -1380,14 +1379,14 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B13" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13">
         <v>-1.5</v>
       </c>
       <c r="E13">
@@ -1434,14 +1433,14 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B14" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14">
         <v>-7</v>
       </c>
       <c r="E14">
@@ -1488,15 +1487,15 @@
         <v>Cowboys</v>
       </c>
     </row>
-    <row r="15" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B15" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="3">
-        <v>8</v>
+      <c r="D15">
+        <v>7.5</v>
       </c>
       <c r="E15">
         <v>7</v>
@@ -1507,7 +1506,7 @@
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
-        <v>-8</v>
+        <v>-7.5</v>
       </c>
       <c r="H15" t="b">
         <f t="shared" si="4"/>
@@ -1527,11 +1526,11 @@
       </c>
       <c r="L15" t="str" cm="1">
         <f t="array" ref="L15">_xlfn.IFS(E15=D15,"No MOV",E15&lt;=0,IF(E15&lt;D15,B15&amp;" "&amp;(D15-E15),C15&amp;" "&amp;(D15-E15)),E15&gt;0,IF(E15&lt;D15,B15&amp;" "&amp;(E15-D15),C15&amp;" "&amp;(E15-D15)))</f>
-        <v>Chiefs -1</v>
+        <v>Chiefs -0.5</v>
       </c>
       <c r="M15" cm="1">
         <f t="array" ref="M15">_xlfn.IFS(E15=D15,"No MOV",E15&lt;0,IF(E15&lt;D15,(D15-E15),(D15-E15)),E15&gt;0,IF(E15&lt;D15,(E15-D15),(E15-D15)))</f>
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="N15" t="str" cm="1">
         <f t="array" ref="N15">IF(J15&lt;&gt;K15,_xlfn.IFS(M15&gt;0,"MAYBE",M15&lt;0,"IGNORE"),"")</f>
@@ -1542,15 +1541,15 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B16" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="3">
-        <v>-4</v>
+      <c r="D16">
+        <v>-4.5</v>
       </c>
       <c r="E16">
         <v>-3</v>
@@ -1561,7 +1560,7 @@
       </c>
       <c r="G16">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="H16" t="b">
         <f t="shared" si="4"/>
@@ -1581,11 +1580,11 @@
       </c>
       <c r="L16" t="str" cm="1">
         <f t="array" ref="L16">_xlfn.IFS(E16=D16,"No MOV",E16&lt;=0,IF(E16&lt;D16,B16&amp;" "&amp;(D16-E16),C16&amp;" "&amp;(D16-E16)),E16&gt;0,IF(E16&lt;D16,B16&amp;" "&amp;(E16-D16),C16&amp;" "&amp;(E16-D16)))</f>
-        <v>Buccaneers -1</v>
+        <v>Buccaneers -1.5</v>
       </c>
       <c r="M16" cm="1">
         <f t="array" ref="M16">_xlfn.IFS(E16=D16,"No MOV",E16&lt;0,IF(E16&lt;D16,(D16-E16),(D16-E16)),E16&gt;0,IF(E16&lt;D16,(E16-D16),(E16-D16)))</f>
-        <v>-1</v>
+        <v>-1.5</v>
       </c>
       <c r="N16" t="str" cm="1">
         <f t="array" ref="N16">IF(J16&lt;&gt;K16,_xlfn.IFS(M16&gt;0,"MAYBE",M16&lt;0,"IGNORE"),"")</f>
@@ -1596,17 +1595,17 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -1659,17 +1658,17 @@
       <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="6" max="9" width="9.28515625" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="3.28515625" customWidth="1"/>
-    <col min="17" max="17" width="2.28515625" customWidth="1"/>
-    <col min="21" max="22" width="2.5703125" customWidth="1"/>
+    <col min="6" max="9" width="9.29296875" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="12.29296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="9.1171875" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="3.29296875" customWidth="1"/>
+    <col min="17" max="17" width="2.29296875" customWidth="1"/>
+    <col min="21" max="22" width="2.5859375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:23" x14ac:dyDescent="0.5">
       <c r="D1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1692,7 +1691,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -1744,7 +1743,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -1812,7 +1811,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B4" t="s">
         <v>28</v>
       </c>
@@ -1869,7 +1868,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -1926,7 +1925,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B6" t="s">
         <v>47</v>
       </c>
@@ -1980,7 +1979,7 @@
         <v>Colts</v>
       </c>
     </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B7" t="s">
         <v>23</v>
       </c>
@@ -2034,7 +2033,7 @@
         <v>Broncos</v>
       </c>
     </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B8" t="s">
         <v>3</v>
       </c>
@@ -2088,7 +2087,7 @@
         <v>Giants</v>
       </c>
     </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -2142,7 +2141,7 @@
         <v>Jaguars</v>
       </c>
     </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B10" t="s">
         <v>26</v>
       </c>
@@ -2196,7 +2195,7 @@
         <v>Bears</v>
       </c>
     </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B11" t="s">
         <v>11</v>
       </c>
@@ -2253,7 +2252,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B12" t="s">
         <v>21</v>
       </c>
@@ -2310,7 +2309,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B13" t="s">
         <v>48</v>
       </c>
@@ -2364,7 +2363,7 @@
         <v>Dolphins</v>
       </c>
     </row>
-    <row r="14" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B14" t="s">
         <v>13</v>
       </c>
@@ -2418,7 +2417,7 @@
         <v>Steelers</v>
       </c>
     </row>
-    <row r="15" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B15" t="s">
         <v>5</v>
       </c>
@@ -2472,7 +2471,7 @@
         <v>Saints</v>
       </c>
     </row>
-    <row r="16" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B16" t="s">
         <v>25</v>
       </c>
@@ -2559,17 +2558,17 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="6" max="9" width="9.28515625" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.29296875" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="12.29296875" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="0" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="3.28515625" customWidth="1"/>
-    <col min="17" max="17" width="2.28515625" customWidth="1"/>
-    <col min="21" max="22" width="2.5703125" customWidth="1"/>
+    <col min="16" max="16" width="3.29296875" customWidth="1"/>
+    <col min="17" max="17" width="2.29296875" customWidth="1"/>
+    <col min="21" max="22" width="2.5859375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:23" x14ac:dyDescent="0.5">
       <c r="D1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2592,7 +2591,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -2644,7 +2643,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -2712,7 +2711,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B4" t="s">
         <v>46</v>
       </c>
@@ -2769,7 +2768,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B5" t="s">
         <v>45</v>
       </c>
@@ -2826,7 +2825,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B6" t="s">
         <v>13</v>
       </c>
@@ -2880,7 +2879,7 @@
         <v>Steelers</v>
       </c>
     </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B7" t="s">
         <v>21</v>
       </c>
@@ -2934,7 +2933,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B8" t="s">
         <v>14</v>
       </c>
@@ -2988,7 +2987,7 @@
         <v>Bengals</v>
       </c>
     </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B9" t="s">
         <v>25</v>
       </c>
@@ -3042,7 +3041,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B10" t="s">
         <v>18</v>
       </c>
@@ -3096,7 +3095,7 @@
         <v>Chiefs</v>
       </c>
     </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B11" t="s">
         <v>27</v>
       </c>
@@ -3153,7 +3152,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B12" t="s">
         <v>20</v>
       </c>
@@ -3207,7 +3206,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B13" t="s">
         <v>24</v>
       </c>
@@ -3261,7 +3260,7 @@
         <v>49ers</v>
       </c>
     </row>
-    <row r="14" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B14" t="s">
         <v>5</v>
       </c>
@@ -3315,7 +3314,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B15" t="s">
         <v>15</v>
       </c>
@@ -3369,7 +3368,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B16" t="s">
         <v>33</v>
       </c>
@@ -3456,20 +3455,20 @@
       <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="4" max="4" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.85546875" customWidth="1"/>
-    <col min="7" max="7" width="6.140625" customWidth="1"/>
-    <col min="8" max="9" width="9.28515625" customWidth="1"/>
-    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" hidden="1" customWidth="1"/>
-    <col min="16" max="17" width="3.140625" customWidth="1"/>
+    <col min="4" max="4" width="4.87890625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.1171875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.87890625" customWidth="1"/>
+    <col min="7" max="7" width="6.1171875" customWidth="1"/>
+    <col min="8" max="9" width="9.29296875" customWidth="1"/>
+    <col min="12" max="12" width="13.87890625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.87890625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="8.703125" hidden="1" customWidth="1"/>
+    <col min="16" max="17" width="3.1171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:23" x14ac:dyDescent="0.5">
       <c r="D1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3492,7 +3491,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -3544,7 +3543,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -3612,7 +3611,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -3669,7 +3668,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -3726,7 +3725,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -3780,7 +3779,7 @@
         <v>Bengals</v>
       </c>
     </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -3834,7 +3833,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B8" t="s">
         <v>13</v>
       </c>
@@ -3888,7 +3887,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B9" t="s">
         <v>15</v>
       </c>
@@ -3942,7 +3941,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B10" t="s">
         <v>17</v>
       </c>
@@ -3996,7 +3995,7 @@
         <v>Bills</v>
       </c>
     </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B11" t="s">
         <v>19</v>
       </c>
@@ -4050,7 +4049,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B12" t="s">
         <v>33</v>
       </c>
@@ -4104,7 +4103,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B13" t="s">
         <v>22</v>
       </c>
@@ -4158,7 +4157,7 @@
         <v>Broncos</v>
       </c>
     </row>
-    <row r="14" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B14" t="s">
         <v>24</v>
       </c>
@@ -4212,7 +4211,7 @@
         <v>49ers</v>
       </c>
     </row>
-    <row r="15" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B15" t="s">
         <v>26</v>
       </c>
@@ -4266,7 +4265,7 @@
         <v>Bears</v>
       </c>
     </row>
-    <row r="16" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:23" x14ac:dyDescent="0.5">
       <c r="B16" t="s">
         <v>28</v>
       </c>
@@ -4354,16 +4353,16 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.42578125" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.87890625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.5859375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.41015625" customWidth="1"/>
+    <col min="14" max="14" width="12.703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.5">
       <c r="C1" t="s">
         <v>53</v>
       </c>
@@ -4377,7 +4376,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.5">
       <c r="C2">
         <v>2</v>
       </c>
@@ -4400,7 +4399,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.5">
       <c r="C3">
         <v>2</v>
       </c>
@@ -4417,7 +4416,7 @@
         <v>0.54999999999999993</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.5">
       <c r="C4">
         <v>10</v>
       </c>
@@ -4440,7 +4439,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.5">
       <c r="C5">
         <v>2</v>
       </c>
@@ -4465,7 +4464,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.5">
       <c r="C6">
         <v>2</v>
       </c>
@@ -4492,7 +4491,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.5">
       <c r="B7" t="s">
         <v>56</v>
       </c>
@@ -4512,7 +4511,7 @@
         <v>0.38596491228070168</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.5">
       <c r="B8" t="s">
         <v>57</v>
       </c>
@@ -4538,7 +4537,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.5">
       <c r="I9" t="s">
         <v>58</v>
       </c>
@@ -4549,7 +4548,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.5">
       <c r="I10" t="s">
         <v>59</v>
       </c>
@@ -4562,7 +4561,7 @@
         <v>0.67567567567567566</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.5">
       <c r="J11">
         <f>J9*J10</f>
         <v>0.32432432432432434</v>
@@ -4580,7 +4579,7 @@
         <v>-1.027027027027027</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.5">
       <c r="J13" t="s">
         <v>54</v>
       </c>
@@ -4588,7 +4587,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.5">
       <c r="I14" t="s">
         <v>58</v>
       </c>
@@ -4599,7 +4598,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.5">
       <c r="I15" t="s">
         <v>59</v>
       </c>
@@ -4612,7 +4611,7 @@
         <v>0.35135135135135132</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.5">
       <c r="J16">
         <f>J14*J15</f>
         <v>0.64864864864864868</v>
@@ -4630,7 +4629,7 @@
         <v>-5.4054054054053946E-2</v>
       </c>
     </row>
-    <row r="18" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="9:14" x14ac:dyDescent="0.5">
       <c r="J18" t="s">
         <v>54</v>
       </c>
@@ -4638,7 +4637,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="9:14" x14ac:dyDescent="0.5">
       <c r="I19" t="s">
         <v>58</v>
       </c>
@@ -4649,7 +4648,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="20" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="9:14" x14ac:dyDescent="0.5">
       <c r="I20" t="s">
         <v>59</v>
       </c>
@@ -4662,7 +4661,7 @@
         <v>0.97222222222222221</v>
       </c>
     </row>
-    <row r="21" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="9:14" x14ac:dyDescent="0.5">
       <c r="J21">
         <f>J19*J20</f>
         <v>0.94444444444444442</v>

</xml_diff>